<commit_message>
add note and some prompt context
</commit_message>
<xml_diff>
--- a/data/guest_information.xlsx
+++ b/data/guest_information.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KenIChi\Chatbot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Mabuchi Motor\MabuchiChatbot\MabuchiChatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41F8F46-6BA3-4527-BFE7-A7326D3DBFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF3D451-CDB1-4D4D-B76C-9C34C4215E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="participants_profile" sheetId="1" r:id="rId1"/>
     <sheet name="department_information" sheetId="2" r:id="rId2"/>
     <sheet name="company_information" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentManualCount="6"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>id</t>
   </si>
@@ -50,84 +50,210 @@
     <t>team</t>
   </si>
   <si>
-    <t>role_level</t>
-  </si>
-  <si>
     <t>seniority_range</t>
   </si>
   <si>
-    <t>fortune_topic</t>
-  </si>
-  <si>
-    <t>tone_preference</t>
-  </si>
-  <si>
     <t>Ken</t>
   </si>
   <si>
-    <t>Kỹ thuật viên bậc 2</t>
-  </si>
-  <si>
-    <t>Viết chương trình AI cho máy ngoại quan Rotor</t>
-  </si>
-  <si>
-    <t>Công việc</t>
-  </si>
-  <si>
-    <t>Hài nhẹ</t>
-  </si>
-  <si>
     <t>Nguyễn Đức Phát</t>
   </si>
   <si>
     <t>&lt;1 năm</t>
   </si>
   <si>
-    <t>Viết chương trình AI cho máy ngoại quan Phủ Sơn</t>
-  </si>
-  <si>
     <t>Hoàng Duy Lộc</t>
   </si>
   <si>
-    <t>Kỹ thuật viên Senior bậc 2 (Nhóm trưởng)</t>
-  </si>
-  <si>
     <t>3 năm</t>
   </si>
   <si>
-    <t>Viết chương trình AI cho máy ngoại quan Hàn Điểm, quản lý các nhóm nghiên cứu kỹ thuật mới</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
     <t>rencent_work_highlight</t>
   </si>
   <si>
-    <t>work_context</t>
-  </si>
-  <si>
     <t>preferred_style</t>
   </si>
   <si>
     <t>Nghiên cứu kĩ thuật mới</t>
   </si>
   <si>
-    <t>current_task</t>
-  </si>
-  <si>
-    <t>Nghiên cứu các kĩ thuật xử lý hình ảnh ứng dụng AI cho việc ngoại quan sản phẩm</t>
+    <t>Tên công ty</t>
+  </si>
+  <si>
+    <t>Mabuchi Motor Việt Nam</t>
+  </si>
+  <si>
+    <t>Lĩnh vực</t>
+  </si>
+  <si>
+    <t>Cột A: ID</t>
+  </si>
+  <si>
+    <t>Cột B: Họ Tên</t>
+  </si>
+  <si>
+    <t>Cột C: Role (Lấy từ ảnh)</t>
+  </si>
+  <si>
+    <t>Cột D: Phòng ban (Map lại)</t>
+  </si>
+  <si>
+    <t>Cột E: Hệ người chơi (Điền thêm)</t>
+  </si>
+  <si>
+    <t>Cột F: Fact Vui (Điền thêm)</t>
+  </si>
+  <si>
+    <t>Đỗ Thanh Đạt</t>
+  </si>
+  <si>
+    <t>GIÁM ĐỐC</t>
+  </si>
+  <si>
+    <t>Ban 2</t>
+  </si>
+  <si>
+    <t>Trùm Cuối</t>
+  </si>
+  <si>
+    <t>Giọng cười vang cả xưởng</t>
+  </si>
+  <si>
+    <t>Phạm Tiến Đạt</t>
+  </si>
+  <si>
+    <t>G/L</t>
+  </si>
+  <si>
+    <t>LK1 (Linh Kiện)</t>
+  </si>
+  <si>
+    <t>Thánh Kaizen</t>
+  </si>
+  <si>
+    <t>Chuyên soi 5S, thấy bụi là ngứa mắt</t>
+  </si>
+  <si>
+    <t>Nguyễn Trần Vĩnh Thắng</t>
+  </si>
+  <si>
+    <t>ENG2</t>
+  </si>
+  <si>
+    <t>LK2</t>
+  </si>
+  <si>
+    <t>Thánh Mò Mẫm</t>
+  </si>
+  <si>
+    <t>Thích tháo máy ra rồi... lắp lại dư ốc</t>
+  </si>
+  <si>
+    <t>Trần Lệ Yến</t>
+  </si>
+  <si>
+    <t>THÔNG DỊCH</t>
+  </si>
+  <si>
+    <t>VP Nghiệp vụ</t>
+  </si>
+  <si>
+    <t>Sứ giả</t>
+  </si>
+  <si>
+    <t>Uống trà sữa thay cơm</t>
+  </si>
+  <si>
+    <t>Khách</t>
+  </si>
+  <si>
+    <t>Hirano San</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>Thích ăn Nem rán</t>
+  </si>
+  <si>
+    <t>roast_level</t>
+  </si>
+  <si>
+    <t>pain_point</t>
+  </si>
+  <si>
+    <t>skill_signature</t>
+  </si>
+  <si>
+    <t>cà khịa vừa</t>
+  </si>
+  <si>
+    <t>cà khịa nhẹ</t>
+  </si>
+  <si>
+    <t>cà khịa mạnh</t>
+  </si>
+  <si>
+    <t>AI, computer vision</t>
+  </si>
+  <si>
+    <t>AI, computer vision, khả năng xử lý tình huống, quản lý đội nhóm</t>
+  </si>
+  <si>
+    <t>AI, computer vision, hát hay</t>
+  </si>
+  <si>
+    <t>Sợ nhất là AI nhìn nhầm bụi thành lỗi, Rotor quay nhanh quá lóa mắt</t>
+  </si>
+  <si>
+    <t>Code chạy được trên máy mình nhưng sang máy Production thì tạch</t>
+  </si>
+  <si>
+    <t>Suốt ngày phải đi giải thích tại sao AI lại "ngu" hơn mắt người</t>
+  </si>
+  <si>
+    <t>newbie</t>
+  </si>
+  <si>
+    <t>exp_level</t>
+  </si>
+  <si>
+    <t>senior, group leader</t>
+  </si>
+  <si>
+    <t>Hà Văn Phú</t>
+  </si>
+  <si>
+    <t>10 năm</t>
+  </si>
+  <si>
+    <t>FH Omron Vision system, làm việc theo kíp sáng/đêm, thần chịch</t>
+  </si>
+  <si>
+    <t>Phải đi ca đêm vừa cô đơn vừa mệt mỏi mà chưa được lên chức Senior</t>
+  </si>
+  <si>
+    <t>làm hơn 10 năm ở công ty nhưng vẫn chưa lên senior, vừa chuyển từ lập trình PLC sang xử lý hình ảnh sử dụng tool FH Omron được 3 năm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -135,7 +261,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -144,6 +270,21 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +295,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,19 +303,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,185 +631,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="3" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.81640625" customWidth="1"/>
-    <col min="7" max="7" width="69.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="80.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="19.81640625" customWidth="1"/>
-    <col min="11" max="11" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.796875" customWidth="1"/>
+    <col min="7" max="7" width="69.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="80.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.796875" customWidth="1"/>
+    <col min="10" max="10" width="20.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>13649</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13654</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13443</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>27</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D13" s="3"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11541</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D13">
@@ -670,9 +844,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.69921875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -681,12 +855,169 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5045E01A-97B7-457A-BA4D-7AF79BFFBD87}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B92D51A-3ADD-487A-B81A-5581A71A39BE}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="83.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>10574</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>12407</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>13611</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>45527</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>